<commit_message>
CIERRE 25 MAYO 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #04  ABRIL 2023/BALANCE  ZAVALETA   ABRIL   2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/CENTRAL #04  ABRIL 2023/BALANCE  ZAVALETA   ABRIL   2023.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21135" windowHeight="11715" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21135" windowHeight="11715" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -291,7 +291,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="501">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1770,6 +1770,30 @@
   </si>
   <si>
     <t xml:space="preserve">ZAVALETA </t>
+  </si>
+  <si>
+    <t>QUESOS-POLLO-LOMOS--JAMON</t>
+  </si>
+  <si>
+    <t>documento</t>
+  </si>
+  <si>
+    <t>quesos-pollo-enchilada</t>
+  </si>
+  <si>
+    <t>Hansel</t>
+  </si>
+  <si>
+    <t>seguros RES</t>
+  </si>
+  <si>
+    <t>FLETE RES</t>
+  </si>
+  <si>
+    <t>Limpieza Trampas</t>
+  </si>
+  <si>
+    <t>Comision Banco</t>
   </si>
 </sst>
 </file>
@@ -3391,7 +3415,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="511">
+  <cellXfs count="518">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4227,6 +4251,39 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="15" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4302,39 +4359,6 @@
     <xf numFmtId="44" fontId="8" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="7" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4401,6 +4425,23 @@
     <xf numFmtId="44" fontId="2" fillId="18" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="76" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -6517,23 +6558,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="482"/>
-      <c r="C1" s="484" t="s">
+      <c r="B1" s="457"/>
+      <c r="C1" s="459" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="485"/>
-      <c r="E1" s="485"/>
-      <c r="F1" s="485"/>
-      <c r="G1" s="485"/>
-      <c r="H1" s="485"/>
-      <c r="I1" s="485"/>
-      <c r="J1" s="485"/>
-      <c r="K1" s="485"/>
-      <c r="L1" s="485"/>
-      <c r="M1" s="485"/>
+      <c r="D1" s="460"/>
+      <c r="E1" s="460"/>
+      <c r="F1" s="460"/>
+      <c r="G1" s="460"/>
+      <c r="H1" s="460"/>
+      <c r="I1" s="460"/>
+      <c r="J1" s="460"/>
+      <c r="K1" s="460"/>
+      <c r="L1" s="460"/>
+      <c r="M1" s="460"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="483"/>
+      <c r="B2" s="458"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -6543,24 +6584,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="486" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="487"/>
+      <c r="B3" s="461" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="462"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="488" t="s">
+      <c r="H3" s="463" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="488"/>
+      <c r="I3" s="463"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="480" t="s">
+      <c r="P3" s="455" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="453" t="s">
+      <c r="R3" s="464" t="s">
         <v>3</v>
       </c>
     </row>
@@ -6575,14 +6616,14 @@
       <c r="D4" s="24">
         <v>44892</v>
       </c>
-      <c r="E4" s="455" t="s">
+      <c r="E4" s="466" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="456"/>
-      <c r="H4" s="457" t="s">
+      <c r="F4" s="467"/>
+      <c r="H4" s="468" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="458"/>
+      <c r="I4" s="469"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -6592,11 +6633,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="481"/>
+      <c r="P4" s="456"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="454"/>
+      <c r="R4" s="465"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -8431,11 +8472,11 @@
       <c r="J49" s="74"/>
       <c r="K49" s="85"/>
       <c r="L49" s="49"/>
-      <c r="M49" s="464">
+      <c r="M49" s="475">
         <f>SUM(M5:M40)</f>
         <v>1399609.5</v>
       </c>
-      <c r="N49" s="464">
+      <c r="N49" s="475">
         <f>SUM(N5:N40)</f>
         <v>910600</v>
       </c>
@@ -8443,7 +8484,7 @@
         <f>SUM(P5:P40)</f>
         <v>3236981.46</v>
       </c>
-      <c r="Q49" s="476">
+      <c r="Q49" s="487">
         <f>SUM(Q5:Q40)</f>
         <v>-199</v>
       </c>
@@ -8464,10 +8505,10 @@
       <c r="J50" s="87"/>
       <c r="K50" s="88"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="465"/>
-      <c r="N50" s="465"/>
+      <c r="M50" s="476"/>
+      <c r="N50" s="476"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="477"/>
+      <c r="Q50" s="488"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>571934</v>
@@ -8522,11 +8563,11 @@
       <c r="J53" s="74"/>
       <c r="K53" s="48"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="478">
+      <c r="M53" s="453">
         <f>M49+N49</f>
         <v>2310209.5</v>
       </c>
-      <c r="N53" s="479"/>
+      <c r="N53" s="454"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -8951,26 +8992,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="472" t="s">
+      <c r="H77" s="483" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="473"/>
+      <c r="I77" s="484"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="474">
+      <c r="K77" s="485">
         <f>I75+L75</f>
         <v>1552957.04</v>
       </c>
-      <c r="L77" s="475"/>
+      <c r="L77" s="486"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="466" t="s">
+      <c r="D78" s="477" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="466"/>
+      <c r="E78" s="477"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>-123007.98000000021</v>
@@ -8979,22 +9020,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="467" t="s">
+      <c r="D79" s="478" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="467"/>
+      <c r="E79" s="478"/>
       <c r="F79" s="101">
         <v>-1513561.68</v>
       </c>
-      <c r="I79" s="468" t="s">
+      <c r="I79" s="479" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="469"/>
-      <c r="K79" s="470">
+      <c r="J79" s="480"/>
+      <c r="K79" s="481">
         <f>F81+F82+F83</f>
         <v>1950142.8099999996</v>
       </c>
-      <c r="L79" s="470"/>
+      <c r="L79" s="481"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -9035,11 +9076,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="471">
+      <c r="K81" s="482">
         <f>-C4</f>
         <v>-3445405.07</v>
       </c>
-      <c r="L81" s="470"/>
+      <c r="L81" s="481"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -9056,22 +9097,22 @@
       <c r="C83" s="172">
         <v>44955</v>
       </c>
-      <c r="D83" s="459" t="s">
+      <c r="D83" s="470" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="460"/>
+      <c r="E83" s="471"/>
       <c r="F83" s="173">
         <v>3504178.07</v>
       </c>
-      <c r="I83" s="461" t="s">
+      <c r="I83" s="472" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="462"/>
-      <c r="K83" s="463">
+      <c r="J83" s="473"/>
+      <c r="K83" s="474">
         <f>K79+K81</f>
         <v>-1495262.2600000002</v>
       </c>
-      <c r="L83" s="463"/>
+      <c r="L83" s="474"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -9218,12 +9259,6 @@
     <sortCondition ref="J33:J44"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -9240,6 +9275,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -11922,23 +11963,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="482"/>
-      <c r="C1" s="484" t="s">
+      <c r="B1" s="457"/>
+      <c r="C1" s="459" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="485"/>
-      <c r="E1" s="485"/>
-      <c r="F1" s="485"/>
-      <c r="G1" s="485"/>
-      <c r="H1" s="485"/>
-      <c r="I1" s="485"/>
-      <c r="J1" s="485"/>
-      <c r="K1" s="485"/>
-      <c r="L1" s="485"/>
-      <c r="M1" s="485"/>
+      <c r="D1" s="460"/>
+      <c r="E1" s="460"/>
+      <c r="F1" s="460"/>
+      <c r="G1" s="460"/>
+      <c r="H1" s="460"/>
+      <c r="I1" s="460"/>
+      <c r="J1" s="460"/>
+      <c r="K1" s="460"/>
+      <c r="L1" s="460"/>
+      <c r="M1" s="460"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="483"/>
+      <c r="B2" s="458"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -11948,24 +11989,24 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="486" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="487"/>
+      <c r="B3" s="461" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="462"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="488" t="s">
+      <c r="H3" s="463" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="488"/>
+      <c r="I3" s="463"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="480" t="s">
+      <c r="P3" s="455" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="453" t="s">
+      <c r="R3" s="464" t="s">
         <v>3</v>
       </c>
     </row>
@@ -11980,14 +12021,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="455" t="s">
+      <c r="E4" s="466" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="456"/>
-      <c r="H4" s="457" t="s">
+      <c r="F4" s="467"/>
+      <c r="H4" s="468" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="458"/>
+      <c r="I4" s="469"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -11997,11 +12038,11 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="481"/>
+      <c r="P4" s="456"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="454"/>
+      <c r="R4" s="465"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
@@ -13977,11 +14018,11 @@
       <c r="L49" s="49">
         <v>5160.4799999999996</v>
       </c>
-      <c r="M49" s="464">
+      <c r="M49" s="475">
         <f>SUM(M5:M40)</f>
         <v>1964337.8699999999</v>
       </c>
-      <c r="N49" s="464">
+      <c r="N49" s="475">
         <f>SUM(N5:N40)</f>
         <v>1314937</v>
       </c>
@@ -13989,7 +14030,7 @@
         <f>SUM(P5:P40)</f>
         <v>3956557.8699999996</v>
       </c>
-      <c r="Q49" s="476">
+      <c r="Q49" s="487">
         <f>SUM(Q5:Q40)</f>
         <v>-996.13000000000466</v>
       </c>
@@ -14022,10 +14063,10 @@
       <c r="L50" s="89">
         <v>4412</v>
       </c>
-      <c r="M50" s="465"/>
-      <c r="N50" s="465"/>
+      <c r="M50" s="476"/>
+      <c r="N50" s="476"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="477"/>
+      <c r="Q50" s="488"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>16567</v>
@@ -14116,11 +14157,11 @@
       <c r="L53" s="49">
         <v>4698</v>
       </c>
-      <c r="M53" s="478">
+      <c r="M53" s="453">
         <f>M49+N49</f>
         <v>3279274.87</v>
       </c>
-      <c r="N53" s="479"/>
+      <c r="N53" s="454"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -14679,26 +14720,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="472" t="s">
+      <c r="H77" s="483" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="473"/>
+      <c r="I77" s="484"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="474">
+      <c r="K77" s="485">
         <f>I75+L75</f>
         <v>526980.64000000013</v>
       </c>
-      <c r="L77" s="475"/>
+      <c r="L77" s="486"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="466" t="s">
+      <c r="D78" s="477" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="466"/>
+      <c r="E78" s="477"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1939381.5999999999</v>
@@ -14707,22 +14748,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="467" t="s">
+      <c r="D79" s="478" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="467"/>
+      <c r="E79" s="478"/>
       <c r="F79" s="101">
         <v>-1830849.67</v>
       </c>
-      <c r="I79" s="468" t="s">
+      <c r="I79" s="479" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="469"/>
-      <c r="K79" s="470">
+      <c r="J79" s="480"/>
+      <c r="K79" s="481">
         <f>F81+F82+F83</f>
         <v>3946521.55</v>
       </c>
-      <c r="L79" s="470"/>
+      <c r="L79" s="481"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -14763,11 +14804,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="471">
+      <c r="K81" s="482">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="470"/>
+      <c r="L81" s="481"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -14784,10 +14825,10 @@
       <c r="C83" s="172">
         <v>44988</v>
       </c>
-      <c r="D83" s="459" t="s">
+      <c r="D83" s="470" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="460"/>
+      <c r="E83" s="471"/>
       <c r="F83" s="173">
         <v>3720574.62</v>
       </c>
@@ -14946,6 +14987,12 @@
     <sortCondition ref="J46:J65"/>
   </sortState>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -14962,12 +15009,6 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -17653,7 +17694,7 @@
   <dimension ref="A1:S105"/>
   <sheetViews>
     <sheetView topLeftCell="A60" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17679,23 +17720,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="482"/>
-      <c r="C1" s="484" t="s">
+      <c r="B1" s="457"/>
+      <c r="C1" s="459" t="s">
         <v>238</v>
       </c>
-      <c r="D1" s="485"/>
-      <c r="E1" s="485"/>
-      <c r="F1" s="485"/>
-      <c r="G1" s="485"/>
-      <c r="H1" s="485"/>
-      <c r="I1" s="485"/>
-      <c r="J1" s="485"/>
-      <c r="K1" s="485"/>
-      <c r="L1" s="485"/>
-      <c r="M1" s="485"/>
+      <c r="D1" s="460"/>
+      <c r="E1" s="460"/>
+      <c r="F1" s="460"/>
+      <c r="G1" s="460"/>
+      <c r="H1" s="460"/>
+      <c r="I1" s="460"/>
+      <c r="J1" s="460"/>
+      <c r="K1" s="460"/>
+      <c r="L1" s="460"/>
+      <c r="M1" s="460"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="483"/>
+      <c r="B2" s="458"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -17705,21 +17746,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="486" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="487"/>
+      <c r="B3" s="461" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="462"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="488" t="s">
+      <c r="H3" s="463" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="488"/>
+      <c r="I3" s="463"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="480" t="s">
+      <c r="P3" s="455" t="s">
         <v>2</v>
       </c>
       <c r="R3" s="509" t="s">
@@ -17737,14 +17778,14 @@
       <c r="D4" s="24">
         <v>44955</v>
       </c>
-      <c r="E4" s="455" t="s">
+      <c r="E4" s="466" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="456"/>
-      <c r="H4" s="457" t="s">
+      <c r="F4" s="467"/>
+      <c r="H4" s="468" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="458"/>
+      <c r="I4" s="469"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -17754,7 +17795,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="481"/>
+      <c r="P4" s="456"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -19739,11 +19780,11 @@
       <c r="L49" s="376">
         <v>6074.64</v>
       </c>
-      <c r="M49" s="464">
+      <c r="M49" s="475">
         <f>SUM(M5:M40)</f>
         <v>1803019.98</v>
       </c>
-      <c r="N49" s="464">
+      <c r="N49" s="475">
         <f>SUM(N5:N40)</f>
         <v>1138524</v>
       </c>
@@ -19751,7 +19792,7 @@
         <f>SUM(P5:P40)</f>
         <v>3684795.48</v>
       </c>
-      <c r="Q49" s="476">
+      <c r="Q49" s="487">
         <f>SUM(Q5:Q40)</f>
         <v>7.9800000000104774</v>
       </c>
@@ -19784,10 +19825,10 @@
       <c r="L50" s="378">
         <v>10278.9</v>
       </c>
-      <c r="M50" s="465"/>
-      <c r="N50" s="465"/>
+      <c r="M50" s="476"/>
+      <c r="N50" s="476"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="477"/>
+      <c r="Q50" s="488"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
         <v>353172.5</v>
@@ -19878,11 +19919,11 @@
       <c r="L53" s="376">
         <v>28000</v>
       </c>
-      <c r="M53" s="478">
+      <c r="M53" s="453">
         <f>M49+N49</f>
         <v>2941543.98</v>
       </c>
-      <c r="N53" s="479"/>
+      <c r="N53" s="454"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
@@ -20361,26 +20402,26 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="472" t="s">
+      <c r="H77" s="483" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="473"/>
+      <c r="I77" s="484"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="474">
+      <c r="K77" s="485">
         <f>I75+L75</f>
         <v>646140.08000000031</v>
       </c>
-      <c r="L77" s="475"/>
+      <c r="L77" s="486"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="466" t="s">
+      <c r="D78" s="477" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="466"/>
+      <c r="E78" s="477"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
         <v>1113109.92</v>
@@ -20389,22 +20430,22 @@
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="467" t="s">
+      <c r="D79" s="478" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="467"/>
+      <c r="E79" s="478"/>
       <c r="F79" s="101">
         <v>-1405309.97</v>
       </c>
-      <c r="I79" s="468" t="s">
+      <c r="I79" s="479" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="469"/>
-      <c r="K79" s="470">
+      <c r="J79" s="480"/>
+      <c r="K79" s="481">
         <f>F81+F82+F83</f>
         <v>3400888.74</v>
       </c>
-      <c r="L79" s="470"/>
+      <c r="L79" s="481"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -20445,11 +20486,11 @@
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="471">
+      <c r="K81" s="482">
         <f>-C4</f>
         <v>-3504178.07</v>
       </c>
-      <c r="L81" s="470"/>
+      <c r="L81" s="481"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -20466,22 +20507,22 @@
       <c r="C83" s="172">
         <v>45014</v>
       </c>
-      <c r="D83" s="459" t="s">
+      <c r="D83" s="470" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="460"/>
+      <c r="E83" s="471"/>
       <c r="F83" s="173">
         <v>3567993.62</v>
       </c>
-      <c r="I83" s="461" t="s">
+      <c r="I83" s="472" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="462"/>
-      <c r="K83" s="463">
+      <c r="J83" s="473"/>
+      <c r="K83" s="474">
         <f>K79+K81</f>
         <v>-103289.32999999961</v>
       </c>
-      <c r="L83" s="463"/>
+      <c r="L83" s="474"/>
     </row>
     <row r="84" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C84" s="174"/>
@@ -20628,12 +20669,6 @@
     <sortCondition ref="J46:J60"/>
   </sortState>
   <mergeCells count="22">
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -20650,6 +20685,12 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -23182,10 +23223,10 @@
   <dimension ref="A1:S105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="F29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="4" topLeftCell="F41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F40" sqref="F40"/>
+      <selection pane="bottomRight" activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -23211,23 +23252,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="482"/>
-      <c r="C1" s="484" t="s">
+      <c r="B1" s="457"/>
+      <c r="C1" s="459" t="s">
         <v>368</v>
       </c>
-      <c r="D1" s="485"/>
-      <c r="E1" s="485"/>
-      <c r="F1" s="485"/>
-      <c r="G1" s="485"/>
-      <c r="H1" s="485"/>
-      <c r="I1" s="485"/>
-      <c r="J1" s="485"/>
-      <c r="K1" s="485"/>
-      <c r="L1" s="485"/>
-      <c r="M1" s="485"/>
+      <c r="D1" s="460"/>
+      <c r="E1" s="460"/>
+      <c r="F1" s="460"/>
+      <c r="G1" s="460"/>
+      <c r="H1" s="460"/>
+      <c r="I1" s="460"/>
+      <c r="J1" s="460"/>
+      <c r="K1" s="460"/>
+      <c r="L1" s="460"/>
+      <c r="M1" s="460"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="483"/>
+      <c r="B2" s="458"/>
       <c r="C2" s="5"/>
       <c r="H2" s="8"/>
       <c r="I2" s="9"/>
@@ -23237,21 +23278,21 @@
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="486" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="487"/>
+      <c r="B3" s="461" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="462"/>
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="488" t="s">
+      <c r="H3" s="463" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="488"/>
+      <c r="I3" s="463"/>
       <c r="K3" s="18"/>
       <c r="L3" s="19"/>
       <c r="M3" s="20"/>
-      <c r="P3" s="480" t="s">
+      <c r="P3" s="455" t="s">
         <v>2</v>
       </c>
       <c r="R3" s="509" t="s">
@@ -23269,14 +23310,14 @@
       <c r="D4" s="24">
         <v>45014</v>
       </c>
-      <c r="E4" s="455" t="s">
+      <c r="E4" s="466" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="456"/>
-      <c r="H4" s="457" t="s">
+      <c r="F4" s="467"/>
+      <c r="H4" s="468" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="458"/>
+      <c r="I4" s="469"/>
       <c r="J4" s="25"/>
       <c r="K4" s="26"/>
       <c r="L4" s="27"/>
@@ -23286,7 +23327,7 @@
       <c r="N4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="481"/>
+      <c r="P4" s="456"/>
       <c r="Q4" s="30" t="s">
         <v>9</v>
       </c>
@@ -24938,36 +24979,50 @@
       <c r="B40" s="32">
         <v>45050</v>
       </c>
-      <c r="C40" s="93"/>
-      <c r="D40" s="94"/>
+      <c r="C40" s="93">
+        <v>8319</v>
+      </c>
+      <c r="D40" s="94" t="s">
+        <v>493</v>
+      </c>
       <c r="E40" s="35">
         <v>45050</v>
       </c>
-      <c r="F40" s="97"/>
+      <c r="F40" s="97">
+        <v>393608</v>
+      </c>
       <c r="G40" s="37"/>
       <c r="H40" s="38">
         <v>45050</v>
       </c>
-      <c r="I40" s="98"/>
-      <c r="J40" s="338"/>
-      <c r="K40" s="343"/>
-      <c r="L40" s="49"/>
+      <c r="I40" s="98">
+        <v>3912</v>
+      </c>
+      <c r="J40" s="338">
+        <v>45050</v>
+      </c>
+      <c r="K40" s="343" t="s">
+        <v>494</v>
+      </c>
+      <c r="L40" s="49">
+        <v>179053.83</v>
+      </c>
       <c r="M40" s="42">
-        <v>0</v>
+        <f>172044+52328.5+3313.2</f>
+        <v>227685.7</v>
       </c>
       <c r="N40" s="43">
-        <v>0</v>
+        <v>43067</v>
       </c>
       <c r="P40" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>462037.53</v>
       </c>
       <c r="Q40" s="45">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R40" s="46">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="R40" s="282">
+        <v>68429.53</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -24975,29 +25030,39 @@
       <c r="B41" s="32">
         <v>45051</v>
       </c>
-      <c r="C41" s="93"/>
-      <c r="D41" s="365"/>
+      <c r="C41" s="93">
+        <f>12164+1225</f>
+        <v>13389</v>
+      </c>
+      <c r="D41" s="511" t="s">
+        <v>495</v>
+      </c>
       <c r="E41" s="35">
         <v>45051</v>
       </c>
-      <c r="F41" s="97"/>
+      <c r="F41" s="97">
+        <v>156015</v>
+      </c>
       <c r="G41" s="37"/>
       <c r="H41" s="38">
         <v>45051</v>
       </c>
-      <c r="I41" s="103"/>
+      <c r="I41" s="103">
+        <v>2267</v>
+      </c>
       <c r="J41" s="338"/>
       <c r="K41" s="347"/>
       <c r="L41" s="49"/>
       <c r="M41" s="42">
-        <v>0</v>
+        <f>66103+799</f>
+        <v>66902</v>
       </c>
       <c r="N41" s="43">
-        <v>0</v>
+        <v>73457</v>
       </c>
       <c r="P41" s="69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>156015</v>
       </c>
       <c r="Q41" s="45">
         <f t="shared" si="1"/>
@@ -25101,9 +25166,15 @@
     </row>
     <row r="45" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="31"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="93"/>
-      <c r="D45" s="102"/>
+      <c r="B45" s="32">
+        <v>45030</v>
+      </c>
+      <c r="C45" s="93">
+        <v>200000</v>
+      </c>
+      <c r="D45" s="102" t="s">
+        <v>232</v>
+      </c>
       <c r="E45" s="35"/>
       <c r="F45" s="97"/>
       <c r="G45" s="37"/>
@@ -25137,9 +25208,15 @@
     </row>
     <row r="46" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="31"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="93"/>
-      <c r="D46" s="102"/>
+      <c r="B46" s="32">
+        <v>45034</v>
+      </c>
+      <c r="C46" s="93">
+        <v>193160.35</v>
+      </c>
+      <c r="D46" s="102" t="s">
+        <v>232</v>
+      </c>
       <c r="E46" s="35"/>
       <c r="F46" s="97"/>
       <c r="G46" s="37"/>
@@ -25176,7 +25253,7 @@
       <c r="B47" s="32">
         <v>45035</v>
       </c>
-      <c r="C47" s="93">
+      <c r="C47" s="513">
         <v>8093</v>
       </c>
       <c r="D47" s="102" t="s">
@@ -25218,7 +25295,7 @@
       <c r="B48" s="32">
         <v>45035</v>
       </c>
-      <c r="C48" s="93">
+      <c r="C48" s="513">
         <v>13752</v>
       </c>
       <c r="D48" s="102" t="s">
@@ -25255,7 +25332,7 @@
       <c r="B49" s="32">
         <v>45035</v>
       </c>
-      <c r="C49" s="93">
+      <c r="C49" s="513">
         <v>1889</v>
       </c>
       <c r="D49" s="403" t="s">
@@ -25275,19 +25352,19 @@
       <c r="L49" s="49">
         <v>25617.51</v>
       </c>
-      <c r="M49" s="464">
+      <c r="M49" s="475">
         <f>SUM(M5:M40)</f>
-        <v>1824079.6</v>
-      </c>
-      <c r="N49" s="464">
+        <v>2051765.3</v>
+      </c>
+      <c r="N49" s="475">
         <f>SUM(N5:N40)</f>
-        <v>1698257</v>
+        <v>1741324</v>
       </c>
       <c r="P49" s="111">
         <f>SUM(P5:P40)</f>
-        <v>4369435.5999999996</v>
-      </c>
-      <c r="Q49" s="476">
+        <v>4831473.13</v>
+      </c>
+      <c r="Q49" s="487">
         <f>SUM(Q5:Q40)</f>
         <v>-111.39999999999418</v>
       </c>
@@ -25300,7 +25377,7 @@
       <c r="B50" s="32">
         <v>45035</v>
       </c>
-      <c r="C50" s="93">
+      <c r="C50" s="513">
         <f>8428+70</f>
         <v>8498</v>
       </c>
@@ -25315,13 +25392,13 @@
       <c r="J50" s="87"/>
       <c r="K50" s="343"/>
       <c r="L50" s="89"/>
-      <c r="M50" s="465"/>
-      <c r="N50" s="465"/>
+      <c r="M50" s="476"/>
+      <c r="N50" s="476"/>
       <c r="P50" s="44"/>
-      <c r="Q50" s="477"/>
+      <c r="Q50" s="488"/>
       <c r="R50" s="112">
         <f>SUM(R5:R49)</f>
-        <v>29443</v>
+        <v>97872.53</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -25329,7 +25406,7 @@
       <c r="B51" s="32">
         <v>45035</v>
       </c>
-      <c r="C51" s="93">
+      <c r="C51" s="513">
         <f>8424+830</f>
         <v>9254</v>
       </c>
@@ -25354,7 +25431,7 @@
       <c r="B52" s="32">
         <v>45035</v>
       </c>
-      <c r="C52" s="93">
+      <c r="C52" s="513">
         <f>2679+1477</f>
         <v>4156</v>
       </c>
@@ -25376,9 +25453,15 @@
     </row>
     <row r="53" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="31"/>
-      <c r="B53" s="32"/>
-      <c r="C53" s="93"/>
-      <c r="D53" s="114"/>
+      <c r="B53" s="32">
+        <v>45044</v>
+      </c>
+      <c r="C53" s="93">
+        <v>200000</v>
+      </c>
+      <c r="D53" s="114" t="s">
+        <v>232</v>
+      </c>
       <c r="E53" s="104"/>
       <c r="F53" s="110"/>
       <c r="G53" s="37"/>
@@ -25387,19 +25470,25 @@
       <c r="J53" s="338"/>
       <c r="K53" s="343"/>
       <c r="L53" s="49"/>
-      <c r="M53" s="478">
+      <c r="M53" s="453">
         <f>M49+N49</f>
-        <v>3522336.6</v>
-      </c>
-      <c r="N53" s="479"/>
+        <v>3793089.3</v>
+      </c>
+      <c r="N53" s="454"/>
       <c r="P53" s="44"/>
       <c r="Q53" s="19"/>
     </row>
     <row r="54" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="31"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="93"/>
-      <c r="D54" s="114"/>
+      <c r="B54" s="32">
+        <v>45048</v>
+      </c>
+      <c r="C54" s="93">
+        <v>406180</v>
+      </c>
+      <c r="D54" s="114" t="s">
+        <v>232</v>
+      </c>
       <c r="E54" s="104"/>
       <c r="F54" s="110"/>
       <c r="G54" s="37"/>
@@ -25423,9 +25512,15 @@
       <c r="G55" s="37"/>
       <c r="H55" s="106"/>
       <c r="I55" s="103"/>
-      <c r="J55" s="338"/>
-      <c r="K55" s="349"/>
-      <c r="L55" s="49"/>
+      <c r="J55" s="338">
+        <v>45028</v>
+      </c>
+      <c r="K55" s="349" t="s">
+        <v>331</v>
+      </c>
+      <c r="L55" s="49">
+        <v>1856</v>
+      </c>
       <c r="M55" s="113"/>
       <c r="N55" s="113"/>
       <c r="P55" s="44"/>
@@ -25441,9 +25536,15 @@
       <c r="G56" s="37"/>
       <c r="H56" s="106"/>
       <c r="I56" s="103"/>
-      <c r="J56" s="341"/>
-      <c r="K56" s="343"/>
-      <c r="L56" s="84"/>
+      <c r="J56" s="341">
+        <v>45030</v>
+      </c>
+      <c r="K56" s="343" t="s">
+        <v>496</v>
+      </c>
+      <c r="L56" s="84">
+        <v>696</v>
+      </c>
       <c r="M56" s="113"/>
       <c r="N56" s="113"/>
       <c r="P56" s="44"/>
@@ -25459,9 +25560,15 @@
       <c r="G57" s="37"/>
       <c r="H57" s="106"/>
       <c r="I57" s="103"/>
-      <c r="J57" s="341"/>
-      <c r="K57" s="343"/>
-      <c r="L57" s="84"/>
+      <c r="J57" s="341">
+        <v>45034</v>
+      </c>
+      <c r="K57" s="343" t="s">
+        <v>497</v>
+      </c>
+      <c r="L57" s="84">
+        <v>3480</v>
+      </c>
       <c r="M57" s="113"/>
       <c r="N57" s="113"/>
       <c r="P57" s="44"/>
@@ -25477,9 +25584,15 @@
       <c r="G58" s="37"/>
       <c r="H58" s="106"/>
       <c r="I58" s="103"/>
-      <c r="J58" s="341"/>
-      <c r="K58" s="343"/>
-      <c r="L58" s="84"/>
+      <c r="J58" s="341">
+        <v>45037</v>
+      </c>
+      <c r="K58" s="343" t="s">
+        <v>498</v>
+      </c>
+      <c r="L58" s="84">
+        <v>28000</v>
+      </c>
       <c r="M58" s="113"/>
       <c r="N58" s="113"/>
       <c r="P58" s="44"/>
@@ -25495,9 +25608,15 @@
       <c r="G59" s="37"/>
       <c r="H59" s="106"/>
       <c r="I59" s="103"/>
-      <c r="J59" s="341"/>
-      <c r="K59" s="343"/>
-      <c r="L59" s="84"/>
+      <c r="J59" s="341">
+        <v>45042</v>
+      </c>
+      <c r="K59" s="343" t="s">
+        <v>497</v>
+      </c>
+      <c r="L59" s="84">
+        <v>3480</v>
+      </c>
       <c r="M59" s="113"/>
       <c r="N59" s="113"/>
       <c r="P59" s="44"/>
@@ -25513,9 +25632,15 @@
       <c r="G60" s="37"/>
       <c r="H60" s="106"/>
       <c r="I60" s="103"/>
-      <c r="J60" s="341"/>
-      <c r="K60" s="343"/>
-      <c r="L60" s="84"/>
+      <c r="J60" s="341">
+        <v>45042</v>
+      </c>
+      <c r="K60" s="343" t="s">
+        <v>228</v>
+      </c>
+      <c r="L60" s="84">
+        <v>1298.04</v>
+      </c>
       <c r="M60" s="113"/>
       <c r="N60" s="113"/>
       <c r="P60" s="44"/>
@@ -25531,9 +25656,15 @@
       <c r="G61" s="37"/>
       <c r="H61" s="106"/>
       <c r="I61" s="103"/>
-      <c r="J61" s="341"/>
-      <c r="K61" s="383"/>
-      <c r="L61" s="84"/>
+      <c r="J61" s="341">
+        <v>45049</v>
+      </c>
+      <c r="K61" s="514" t="s">
+        <v>225</v>
+      </c>
+      <c r="L61" s="84">
+        <v>1098</v>
+      </c>
       <c r="M61" s="113"/>
       <c r="N61" s="113"/>
       <c r="P61" s="44"/>
@@ -25549,9 +25680,15 @@
       <c r="G62" s="37"/>
       <c r="H62" s="106"/>
       <c r="I62" s="103"/>
-      <c r="J62" s="341"/>
-      <c r="K62" s="350"/>
-      <c r="L62" s="84"/>
+      <c r="J62" s="341">
+        <v>45051</v>
+      </c>
+      <c r="K62" s="350" t="s">
+        <v>498</v>
+      </c>
+      <c r="L62" s="84">
+        <v>28000</v>
+      </c>
       <c r="M62" s="113"/>
       <c r="N62" s="113"/>
       <c r="P62" s="44"/>
@@ -25567,9 +25704,15 @@
       <c r="G63" s="37"/>
       <c r="H63" s="106"/>
       <c r="I63" s="103"/>
-      <c r="J63" s="341"/>
-      <c r="K63" s="343"/>
-      <c r="L63" s="84"/>
+      <c r="J63" s="341">
+        <v>45051</v>
+      </c>
+      <c r="K63" s="343" t="s">
+        <v>499</v>
+      </c>
+      <c r="L63" s="84">
+        <v>850</v>
+      </c>
       <c r="M63" s="113"/>
       <c r="N63" s="113"/>
       <c r="P63" s="44"/>
@@ -25585,9 +25728,15 @@
       <c r="G64" s="37"/>
       <c r="H64" s="106"/>
       <c r="I64" s="103"/>
-      <c r="J64" s="341"/>
-      <c r="K64" s="350"/>
-      <c r="L64" s="84"/>
+      <c r="J64" s="515">
+        <v>45051</v>
+      </c>
+      <c r="K64" s="516" t="s">
+        <v>500</v>
+      </c>
+      <c r="L64" s="517">
+        <v>47106.080000000002</v>
+      </c>
       <c r="M64" s="113"/>
       <c r="N64" s="113"/>
       <c r="P64" s="44"/>
@@ -25774,7 +25923,7 @@
       </c>
       <c r="C75" s="141">
         <f>SUM(C5:C68)</f>
-        <v>652882</v>
+        <v>1673930.35</v>
       </c>
       <c r="D75" s="142"/>
       <c r="E75" s="143" t="s">
@@ -25782,7 +25931,7 @@
       </c>
       <c r="F75" s="144">
         <f>SUM(F5:F68)</f>
-        <v>4349104</v>
+        <v>4898727</v>
       </c>
       <c r="G75" s="145"/>
       <c r="H75" s="143" t="s">
@@ -25790,7 +25939,7 @@
       </c>
       <c r="I75" s="146">
         <f>SUM(I5:I68)</f>
-        <v>88471</v>
+        <v>94650</v>
       </c>
       <c r="J75" s="147"/>
       <c r="K75" s="148" t="s">
@@ -25798,7 +25947,7 @@
       </c>
       <c r="L75" s="149">
         <f>SUM(L5:L73)-L26</f>
-        <v>278904.52</v>
+        <v>573822.46999999986</v>
       </c>
       <c r="M75" s="150"/>
       <c r="N75" s="150"/>
@@ -25816,50 +25965,50 @@
       <c r="A77" s="152"/>
       <c r="B77" s="153"/>
       <c r="C77" s="1"/>
-      <c r="H77" s="472" t="s">
+      <c r="H77" s="483" t="s">
         <v>15</v>
       </c>
-      <c r="I77" s="473"/>
+      <c r="I77" s="484"/>
       <c r="J77" s="154"/>
-      <c r="K77" s="474">
+      <c r="K77" s="485">
         <f>I75+L75</f>
-        <v>367375.52</v>
-      </c>
-      <c r="L77" s="475"/>
+        <v>668472.46999999986</v>
+      </c>
+      <c r="L77" s="486"/>
       <c r="M77" s="155"/>
       <c r="N77" s="155"/>
       <c r="P77" s="44"/>
       <c r="Q77" s="19"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D78" s="466" t="s">
+      <c r="D78" s="477" t="s">
         <v>16</v>
       </c>
-      <c r="E78" s="466"/>
+      <c r="E78" s="477"/>
       <c r="F78" s="156">
         <f>F75-K77-C75</f>
-        <v>3328846.48</v>
+        <v>2556324.1800000002</v>
       </c>
       <c r="I78" s="157"/>
       <c r="J78" s="158"/>
     </row>
     <row r="79" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D79" s="467" t="s">
+      <c r="D79" s="478" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="467"/>
+      <c r="E79" s="478"/>
       <c r="F79" s="101">
         <v>-2011533.7</v>
       </c>
-      <c r="I79" s="468" t="s">
+      <c r="I79" s="479" t="s">
         <v>18</v>
       </c>
-      <c r="J79" s="469"/>
-      <c r="K79" s="470">
+      <c r="J79" s="480"/>
+      <c r="K79" s="481">
         <f>F81+F82+F83</f>
-        <v>4382596.57</v>
-      </c>
-      <c r="L79" s="470"/>
+        <v>3621899.2700000005</v>
+      </c>
+      <c r="L79" s="481"/>
       <c r="M79" s="159"/>
       <c r="N79" s="159"/>
       <c r="O79" s="160"/>
@@ -25893,18 +26042,18 @@
       </c>
       <c r="F81" s="150">
         <f>SUM(F78:F80)</f>
-        <v>1317312.78</v>
+        <v>544790.48000000021</v>
       </c>
       <c r="H81" s="168"/>
       <c r="I81" s="169" t="s">
         <v>21</v>
       </c>
       <c r="J81" s="170"/>
-      <c r="K81" s="471">
+      <c r="K81" s="482">
         <f>-C4</f>
         <v>-3567993.62</v>
       </c>
-      <c r="L81" s="470"/>
+      <c r="L81" s="481"/>
     </row>
     <row r="82" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D82" s="171" t="s">
@@ -25914,17 +26063,17 @@
         <v>23</v>
       </c>
       <c r="F82" s="101">
-        <v>0</v>
+        <v>11825</v>
       </c>
     </row>
     <row r="83" spans="2:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C83" s="172">
         <v>45051</v>
       </c>
-      <c r="D83" s="459" t="s">
+      <c r="D83" s="470" t="s">
         <v>24</v>
       </c>
-      <c r="E83" s="460"/>
+      <c r="E83" s="471"/>
       <c r="F83" s="173">
         <v>3065283.79</v>
       </c>
@@ -25934,7 +26083,7 @@
       <c r="J83" s="505"/>
       <c r="K83" s="506">
         <f>K79+K81</f>
-        <v>814602.95000000019</v>
+        <v>53905.650000000373</v>
       </c>
       <c r="L83" s="506"/>
     </row>
@@ -25982,6 +26131,7 @@
       <c r="B89" s="181"/>
       <c r="C89" s="185"/>
       <c r="E89" s="44"/>
+      <c r="F89" s="186"/>
       <c r="M89" s="1"/>
     </row>
     <row r="90" spans="2:14" x14ac:dyDescent="0.25">
@@ -25989,7 +26139,7 @@
       <c r="C90" s="185"/>
       <c r="D90" s="188"/>
       <c r="E90" s="44"/>
-      <c r="F90" s="189"/>
+      <c r="F90" s="44"/>
       <c r="M90" s="1"/>
     </row>
     <row r="91" spans="2:14" x14ac:dyDescent="0.25">
@@ -26013,19 +26163,19 @@
     <row r="94" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D94" s="188"/>
       <c r="E94" s="190"/>
-      <c r="F94" s="44"/>
+      <c r="F94" s="512"/>
       <c r="M94" s="1"/>
     </row>
     <row r="95" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D95" s="188"/>
       <c r="E95" s="190"/>
-      <c r="F95" s="44"/>
+      <c r="F95" s="512"/>
       <c r="M95" s="1"/>
     </row>
     <row r="96" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D96" s="188"/>
       <c r="E96" s="190"/>
-      <c r="F96" s="44"/>
+      <c r="F96" s="512"/>
       <c r="M96" s="1"/>
     </row>
     <row r="97" spans="4:13" x14ac:dyDescent="0.25">
@@ -26080,6 +26230,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="M53:N53"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="H4:I4"/>
@@ -26096,12 +26252,6 @@
     <mergeCell ref="H77:I77"/>
     <mergeCell ref="K77:L77"/>
     <mergeCell ref="Q49:Q50"/>
-    <mergeCell ref="M53:N53"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -26118,10 +26268,10 @@
   <dimension ref="A1:N123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F76" sqref="F76"/>
+      <selection pane="bottomRight" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>